<commit_message>
fix dummies and create main labels
</commit_message>
<xml_diff>
--- a/Documentation/variables_codebook.xlsx
+++ b/Documentation/variables_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Github\World Bank\Devolve\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD13696E-66CE-4099-8ABB-DC43BD932CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BB8E95-61A1-4D70-8E2F-9BE6E0B76F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,28 @@
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="choices_current" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$I$238</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="385">
   <si>
     <t>name</t>
   </si>
@@ -900,9 +916,6 @@
     <t>Interruped questionairy</t>
   </si>
   <si>
-    <t>Age &gt; 18 yrs old</t>
-  </si>
-  <si>
     <t>Concent recording</t>
   </si>
   <si>
@@ -910,13 +923,283 @@
   </si>
   <si>
     <t>Interview ID</t>
+  </si>
+  <si>
+    <t>How the interviewee found out about the program</t>
+  </si>
+  <si>
+    <t>Other response for DEVPAR02</t>
+  </si>
+  <si>
+    <t>Who are the other program participants the interviewee knows</t>
+  </si>
+  <si>
+    <t>Other response to the previous question</t>
+  </si>
+  <si>
+    <t>Question about the frequency of Devolve-ICMS deposits</t>
+  </si>
+  <si>
+    <t>Statement about the minimum deposit amount</t>
+  </si>
+  <si>
+    <t>Statement about the relationship between CPF on the receipt and the amount received</t>
+  </si>
+  <si>
+    <t>What happens to unused money on the Cartão Cidadão</t>
+  </si>
+  <si>
+    <t>Which payment methods the interviewee uses</t>
+  </si>
+  <si>
+    <t>What is the most convenient payment method</t>
+  </si>
+  <si>
+    <t>How many times they paid with cash in the last week</t>
+  </si>
+  <si>
+    <t>If the interviewee or their family has a bank account</t>
+  </si>
+  <si>
+    <t>Which banks or financial institutions the family has accounts at</t>
+  </si>
+  <si>
+    <t>If the store they shop at most gives a receipt</t>
+  </si>
+  <si>
+    <t>Reason for shopping at a store that doesn't give a receipt</t>
+  </si>
+  <si>
+    <t>Proportion of purchases at stores that ask for CPF on the receipt</t>
+  </si>
+  <si>
+    <t>Which CPF is used on receipts</t>
+  </si>
+  <si>
+    <t>Frequency of including another person's CPF on the receipt</t>
+  </si>
+  <si>
+    <t>Frequency with which attendants ask about the CPF</t>
+  </si>
+  <si>
+    <t>Frequency of including their own CPF on the receipt when asked</t>
+  </si>
+  <si>
+    <t>Reasons for not putting CPF on the receipt when asked</t>
+  </si>
+  <si>
+    <t>Frequency of asking to include CPF when not asked</t>
+  </si>
+  <si>
+    <t>Reasons for not asking to include CPF on receipts</t>
+  </si>
+  <si>
+    <t>Approximate monthly spending on family purchases</t>
+  </si>
+  <si>
+    <t>Recording the value in full</t>
+  </si>
+  <si>
+    <t>Approximate monthly spending on family purchases, with value range options</t>
+  </si>
+  <si>
+    <t>If the interviewee has the Cartão Cidadão</t>
+  </si>
+  <si>
+    <t>Frequency of including CPF on the receipt currently</t>
+  </si>
+  <si>
+    <t>How long it takes to spend the money from the Devolve card</t>
+  </si>
+  <si>
+    <t>How much of the Cartão Cidadão money is used</t>
+  </si>
+  <si>
+    <t>Main use of the Cartão Cidadão Devolve ICMS</t>
+  </si>
+  <si>
+    <t>If they have had problems using the Cartão Cidadão</t>
+  </si>
+  <si>
+    <t>Problems encountered when using the Cartão Cidadão</t>
+  </si>
+  <si>
+    <t>Reasons for not having picked up the card</t>
+  </si>
+  <si>
+    <t>Concern about the lack of nearby stores that accept the card</t>
+  </si>
+  <si>
+    <t>Concern about knowing how to use the card</t>
+  </si>
+  <si>
+    <t>Concern about someone else in the household using the card</t>
+  </si>
+  <si>
+    <t>Reason why they could not get the card</t>
+  </si>
+  <si>
+    <t>Opinion on income inequality in Brazil</t>
+  </si>
+  <si>
+    <t>Opinion on the government taxing the rich more</t>
+  </si>
+  <si>
+    <t>Opinion on taxes on what is earned vs. what is bought</t>
+  </si>
+  <si>
+    <t>Opinion on paying less taxes on essential goods</t>
+  </si>
+  <si>
+    <t>Value of the ICMS charged in Rio Grande do Sul</t>
+  </si>
+  <si>
+    <t>Value of the ICMS charged in Rio Grande do Sul, with value ranges</t>
+  </si>
+  <si>
+    <t>Opinion on the rule of including CPF to receive more money from the program</t>
+  </si>
+  <si>
+    <t>Position on increasing the tax on food</t>
+  </si>
+  <si>
+    <t>Position on increasing the tax on food with a refund for Devolve participants</t>
+  </si>
+  <si>
+    <t>Position on increasing the tax on food with a refund for all residents of RS</t>
+  </si>
+  <si>
+    <t>Position on decreasing the tax on perfumes and makeup</t>
+  </si>
+  <si>
+    <t>If they know the Nota Fiscal Gaúcha program</t>
+  </si>
+  <si>
+    <t>If they participate in the Nota Fiscal Gaúcha program</t>
+  </si>
+  <si>
+    <t>Main reason for not participating in the Nota Fiscal Gaúcha program</t>
+  </si>
+  <si>
+    <t>Last digit of the phone number dialed by the interviewer</t>
+  </si>
+  <si>
+    <t>If they would like to receive information on how to register for the program</t>
+  </si>
+  <si>
+    <t>Preference for receiving information via SMS or Whatsapp</t>
+  </si>
+  <si>
+    <t>Municipality of residence</t>
+  </si>
+  <si>
+    <t>Age of the interviewee</t>
+  </si>
+  <si>
+    <t>Gender of the interviewee</t>
+  </si>
+  <si>
+    <t>Family's monthly income, including benefits</t>
+  </si>
+  <si>
+    <t>Number of people in the household</t>
+  </si>
+  <si>
+    <t>If the family was affected by the floods</t>
+  </si>
+  <si>
+    <t>Assessment of the impact of the floods on the interviewee's life</t>
+  </si>
+  <si>
+    <t>If they had to leave home during the floods</t>
+  </si>
+  <si>
+    <t>How many days they could not enter their home</t>
+  </si>
+  <si>
+    <t>If they received any help to recover from the floods</t>
+  </si>
+  <si>
+    <t>Type of assistance or help received after the floods</t>
+  </si>
+  <si>
+    <t>Call status</t>
+  </si>
+  <si>
+    <t>Primary key</t>
+  </si>
+  <si>
+    <t>Other response to the DEV04 question</t>
+  </si>
+  <si>
+    <t>Question about all the requirements to participate in the Devolve-ICMS program</t>
+  </si>
+  <si>
+    <t>Other response to the DEV08 question</t>
+  </si>
+  <si>
+    <t>Other response to the PAG03 question</t>
+  </si>
+  <si>
+    <t>Other response to the NFI01a question</t>
+  </si>
+  <si>
+    <t>Other response to the NFI03 question</t>
+  </si>
+  <si>
+    <t>Other response to the NFI04a1 question</t>
+  </si>
+  <si>
+    <t>Other response to the CCD07 question</t>
+  </si>
+  <si>
+    <t>If the person has ever tried to get the Cartão Cidadão</t>
+  </si>
+  <si>
+    <t>Other response to the CCD09 question</t>
+  </si>
+  <si>
+    <t>Other response to the NFG02A question</t>
+  </si>
+  <si>
+    <t>Other response to the INU04a question</t>
+  </si>
+  <si>
+    <t>Strata</t>
+  </si>
+  <si>
+    <t>If the interviewee wants a copy of the consent</t>
+  </si>
+  <si>
+    <t>If the interviewee prefers to receive the copy via SMS or Whatsapp</t>
+  </si>
+  <si>
+    <t>If the interviewee knows the Devolve-ICMS program</t>
+  </si>
+  <si>
+    <t>If the interviewee's family participates in the program</t>
+  </si>
+  <si>
+    <t>If the interviewee knows other program participants</t>
+  </si>
+  <si>
+    <t>If the person has more than 18 years old</t>
+  </si>
+  <si>
+    <t>If the person consents with the continuation of the interview</t>
+  </si>
+  <si>
+    <t>If there is any adult close able to talk that lives in the house</t>
+  </si>
+  <si>
+    <t>If the person is the adult responsible for the decisions in the household or if they could call the responsible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -930,6 +1213,11 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -953,10 +1241,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,13 +1582,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" customWidth="1"/>
     <col min="5" max="6" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1381,7 +1670,7 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>260</v>
@@ -1410,7 +1699,7 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
         <v>260</v>
@@ -1439,7 +1728,7 @@
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>261</v>
@@ -1456,7 +1745,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1468,7 +1757,7 @@
         <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>262</v>
@@ -1485,7 +1774,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -1497,7 +1786,7 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
         <v>261</v>
@@ -1526,7 +1815,7 @@
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>261</v>
@@ -1543,7 +1832,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1555,7 +1844,7 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
@@ -1584,7 +1873,7 @@
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -1613,7 +1902,7 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
         <v>261</v>
@@ -1642,7 +1931,7 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
         <v>261</v>
@@ -1671,7 +1960,7 @@
         <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
         <v>261</v>
@@ -1700,7 +1989,7 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -1716,8 +2005,8 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>292</v>
+      <c r="B15" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1729,7 +2018,7 @@
         <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
@@ -1758,7 +2047,7 @@
         <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
         <v>261</v>
@@ -1787,7 +2076,7 @@
         <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
         <v>263</v>
@@ -1803,20 +2092,20 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
+      <c r="B18" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
-      <c r="D18" t="s">
-        <v>20</v>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
@@ -1832,20 +2121,20 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
+      <c r="B19" s="2" t="s">
+        <v>384</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D19" t="s">
-        <v>20</v>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E19" t="s">
         <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
@@ -1874,7 +2163,7 @@
         <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
         <v>261</v>
@@ -1903,7 +2192,7 @@
         <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
@@ -1932,7 +2221,7 @@
         <v>41</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G22" t="s">
         <v>261</v>
@@ -1948,20 +2237,20 @@
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
-        <v>20</v>
+      <c r="B23" s="2" t="s">
+        <v>382</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
-        <v>20</v>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
@@ -1990,7 +2279,7 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
         <v>261</v>
@@ -2019,7 +2308,7 @@
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
         <v>263</v>
@@ -2048,7 +2337,7 @@
         <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s">
         <v>261</v>
@@ -2077,7 +2366,7 @@
         <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="G27" t="s">
         <v>263</v>
@@ -2093,20 +2382,20 @@
       <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
-        <v>20</v>
+      <c r="B28" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
       </c>
-      <c r="D28" t="s">
-        <v>20</v>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
@@ -2122,20 +2411,20 @@
       <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
-        <v>20</v>
+      <c r="B29" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="D29" t="s">
-        <v>20</v>
+      <c r="D29" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E29" t="s">
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
@@ -2164,7 +2453,7 @@
         <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="G30" t="s">
         <v>261</v>
@@ -2180,20 +2469,20 @@
       <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
+      <c r="B31" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
       </c>
-      <c r="D31" t="s">
-        <v>20</v>
+      <c r="D31" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E31" t="s">
         <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G31" t="s">
         <v>263</v>
@@ -2222,7 +2511,7 @@
         <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="G32" t="s">
         <v>261</v>
@@ -2251,7 +2540,7 @@
         <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="G33" t="s">
         <v>263</v>
@@ -2267,20 +2556,18 @@
       <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="B34" t="s">
-        <v>20</v>
+      <c r="B34" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
       </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" t="s">
         <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="G34" t="s">
         <v>263</v>
@@ -2297,7 +2584,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>295</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
@@ -2309,7 +2596,7 @@
         <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="G35" t="s">
         <v>263</v>
@@ -2325,8 +2612,8 @@
       <c r="A36" t="s">
         <v>20</v>
       </c>
-      <c r="B36" t="s">
-        <v>20</v>
+      <c r="B36" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="C36" t="s">
         <v>20</v>
@@ -2338,7 +2625,7 @@
         <v>55</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G36" t="s">
         <v>264</v>
@@ -2354,20 +2641,20 @@
       <c r="A37" t="s">
         <v>20</v>
       </c>
-      <c r="B37" t="s">
-        <v>20</v>
+      <c r="B37" s="2" t="s">
+        <v>380</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
       </c>
-      <c r="D37" t="s">
-        <v>20</v>
+      <c r="D37" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E37" t="s">
         <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="G37" t="s">
         <v>263</v>
@@ -2383,8 +2670,8 @@
       <c r="A38" t="s">
         <v>20</v>
       </c>
-      <c r="B38" t="s">
-        <v>20</v>
+      <c r="B38" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="C38" t="s">
         <v>20</v>
@@ -2396,7 +2683,7 @@
         <v>57</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="G38" t="s">
         <v>265</v>
@@ -2425,7 +2712,7 @@
         <v>58</v>
       </c>
       <c r="F39" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
@@ -2454,7 +2741,7 @@
         <v>59</v>
       </c>
       <c r="F40" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
@@ -2483,7 +2770,7 @@
         <v>60</v>
       </c>
       <c r="F41" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
@@ -2512,7 +2799,7 @@
         <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="G42" t="s">
         <v>5</v>
@@ -2541,7 +2828,7 @@
         <v>62</v>
       </c>
       <c r="F43" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
@@ -2570,7 +2857,7 @@
         <v>63</v>
       </c>
       <c r="F44" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="G44" t="s">
         <v>5</v>
@@ -2599,7 +2886,7 @@
         <v>64</v>
       </c>
       <c r="F45" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="G45" t="s">
         <v>266</v>
@@ -2628,7 +2915,7 @@
         <v>65</v>
       </c>
       <c r="F46" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="G46" t="s">
         <v>261</v>
@@ -2657,7 +2944,7 @@
         <v>66</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="G47" t="s">
         <v>263</v>
@@ -2686,7 +2973,7 @@
         <v>67</v>
       </c>
       <c r="F48" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="G48" t="s">
         <v>261</v>
@@ -2715,7 +3002,7 @@
         <v>68</v>
       </c>
       <c r="F49" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="G49" t="s">
         <v>263</v>
@@ -2744,7 +3031,7 @@
         <v>69</v>
       </c>
       <c r="F50" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="G50" t="s">
         <v>267</v>
@@ -2760,8 +3047,8 @@
       <c r="A51" t="s">
         <v>20</v>
       </c>
-      <c r="B51" t="s">
-        <v>20</v>
+      <c r="B51" s="2" t="s">
+        <v>364</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -2773,7 +3060,7 @@
         <v>70</v>
       </c>
       <c r="F51" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="G51" t="s">
         <v>263</v>
@@ -2789,8 +3076,8 @@
       <c r="A52" t="s">
         <v>20</v>
       </c>
-      <c r="B52" t="s">
-        <v>20</v>
+      <c r="B52" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="C52" t="s">
         <v>20</v>
@@ -2802,7 +3089,7 @@
         <v>71</v>
       </c>
       <c r="F52" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G52" t="s">
         <v>268</v>
@@ -2819,7 +3106,7 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>299</v>
       </c>
       <c r="C53" t="s">
         <v>20</v>
@@ -2831,7 +3118,7 @@
         <v>72</v>
       </c>
       <c r="F53" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="G53" t="s">
         <v>5</v>
@@ -2860,7 +3147,7 @@
         <v>73</v>
       </c>
       <c r="F54" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="G54" t="s">
         <v>261</v>
@@ -2877,7 +3164,7 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="C55" t="s">
         <v>20</v>
@@ -2889,7 +3176,7 @@
         <v>74</v>
       </c>
       <c r="F55" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="G55" t="s">
         <v>263</v>
@@ -2906,7 +3193,7 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>301</v>
       </c>
       <c r="C56" t="s">
         <v>20</v>
@@ -2918,7 +3205,7 @@
         <v>75</v>
       </c>
       <c r="F56" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="G56" t="s">
         <v>263</v>
@@ -2947,7 +3234,7 @@
         <v>76</v>
       </c>
       <c r="F57" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="G57" t="s">
         <v>261</v>
@@ -2976,7 +3263,7 @@
         <v>77</v>
       </c>
       <c r="F58" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="G58" t="s">
         <v>263</v>
@@ -2993,7 +3280,7 @@
         <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>302</v>
       </c>
       <c r="C59" t="s">
         <v>20</v>
@@ -3005,7 +3292,7 @@
         <v>78</v>
       </c>
       <c r="F59" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="G59" t="s">
         <v>263</v>
@@ -3021,8 +3308,8 @@
       <c r="A60" t="s">
         <v>20</v>
       </c>
-      <c r="B60" t="s">
-        <v>20</v>
+      <c r="B60" s="2" t="s">
+        <v>365</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>
@@ -3034,7 +3321,7 @@
         <v>79</v>
       </c>
       <c r="F60" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="G60" t="s">
         <v>269</v>
@@ -3063,7 +3350,7 @@
         <v>80</v>
       </c>
       <c r="F61" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="G61" t="s">
         <v>261</v>
@@ -3080,7 +3367,7 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>303</v>
       </c>
       <c r="C62" t="s">
         <v>20</v>
@@ -3092,7 +3379,7 @@
         <v>81</v>
       </c>
       <c r="F62" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="G62" t="s">
         <v>265</v>
@@ -3108,9 +3395,6 @@
       <c r="A63" t="s">
         <v>20</v>
       </c>
-      <c r="B63" t="s">
-        <v>20</v>
-      </c>
       <c r="C63" t="s">
         <v>20</v>
       </c>
@@ -3121,7 +3405,7 @@
         <v>82</v>
       </c>
       <c r="F63" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="G63" t="s">
         <v>5</v>
@@ -3150,7 +3434,7 @@
         <v>83</v>
       </c>
       <c r="F64" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="G64" t="s">
         <v>5</v>
@@ -3179,7 +3463,7 @@
         <v>84</v>
       </c>
       <c r="F65" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="G65" t="s">
         <v>5</v>
@@ -3208,7 +3492,7 @@
         <v>85</v>
       </c>
       <c r="F66" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="G66" t="s">
         <v>5</v>
@@ -3237,7 +3521,7 @@
         <v>86</v>
       </c>
       <c r="F67" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="G67" t="s">
         <v>5</v>
@@ -3266,7 +3550,7 @@
         <v>87</v>
       </c>
       <c r="F68" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="G68" t="s">
         <v>5</v>
@@ -3295,7 +3579,7 @@
         <v>88</v>
       </c>
       <c r="F69" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="G69" t="s">
         <v>5</v>
@@ -3312,7 +3596,7 @@
         <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>20</v>
+        <v>304</v>
       </c>
       <c r="C70" t="s">
         <v>20</v>
@@ -3324,7 +3608,7 @@
         <v>89</v>
       </c>
       <c r="F70" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="G70" t="s">
         <v>263</v>
@@ -3341,7 +3625,7 @@
         <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>305</v>
       </c>
       <c r="C71" t="s">
         <v>20</v>
@@ -3353,7 +3637,7 @@
         <v>90</v>
       </c>
       <c r="F71" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="G71" t="s">
         <v>263</v>
@@ -3382,7 +3666,7 @@
         <v>91</v>
       </c>
       <c r="F72" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="G72" t="s">
         <v>261</v>
@@ -3411,7 +3695,7 @@
         <v>92</v>
       </c>
       <c r="F73" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="G73" t="s">
         <v>263</v>
@@ -3428,7 +3712,7 @@
         <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>306</v>
       </c>
       <c r="C74" t="s">
         <v>20</v>
@@ -3440,7 +3724,7 @@
         <v>93</v>
       </c>
       <c r="F74" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="G74" t="s">
         <v>263</v>
@@ -3457,7 +3741,7 @@
         <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>20</v>
+        <v>307</v>
       </c>
       <c r="C75" t="s">
         <v>20</v>
@@ -3469,7 +3753,7 @@
         <v>94</v>
       </c>
       <c r="F75" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="G75" t="s">
         <v>270</v>
@@ -3485,9 +3769,6 @@
       <c r="A76" t="s">
         <v>20</v>
       </c>
-      <c r="B76" t="s">
-        <v>20</v>
-      </c>
       <c r="C76" t="s">
         <v>20</v>
       </c>
@@ -3498,7 +3779,7 @@
         <v>95</v>
       </c>
       <c r="F76" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="G76" t="s">
         <v>5</v>
@@ -3527,7 +3808,7 @@
         <v>96</v>
       </c>
       <c r="F77" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="G77" t="s">
         <v>5</v>
@@ -3556,7 +3837,7 @@
         <v>97</v>
       </c>
       <c r="F78" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="G78" t="s">
         <v>5</v>
@@ -3585,7 +3866,7 @@
         <v>98</v>
       </c>
       <c r="F79" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="G79" t="s">
         <v>5</v>
@@ -3614,7 +3895,7 @@
         <v>99</v>
       </c>
       <c r="F80" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="G80" t="s">
         <v>5</v>
@@ -3643,7 +3924,7 @@
         <v>100</v>
       </c>
       <c r="F81" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G81" t="s">
         <v>5</v>
@@ -3672,7 +3953,7 @@
         <v>101</v>
       </c>
       <c r="F82" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="G82" t="s">
         <v>5</v>
@@ -3701,7 +3982,7 @@
         <v>102</v>
       </c>
       <c r="F83" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="G83" t="s">
         <v>5</v>
@@ -3730,7 +4011,7 @@
         <v>103</v>
       </c>
       <c r="F84" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="G84" t="s">
         <v>5</v>
@@ -3759,7 +4040,7 @@
         <v>104</v>
       </c>
       <c r="F85" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="G85" t="s">
         <v>5</v>
@@ -3788,7 +4069,7 @@
         <v>105</v>
       </c>
       <c r="F86" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="G86" t="s">
         <v>5</v>
@@ -3817,7 +4098,7 @@
         <v>106</v>
       </c>
       <c r="F87" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="G87" t="s">
         <v>5</v>
@@ -3846,7 +4127,7 @@
         <v>107</v>
       </c>
       <c r="F88" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="G88" t="s">
         <v>5</v>
@@ -3875,7 +4156,7 @@
         <v>108</v>
       </c>
       <c r="F89" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="G89" t="s">
         <v>5</v>
@@ -3904,7 +4185,7 @@
         <v>109</v>
       </c>
       <c r="F90" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c r="G90" t="s">
         <v>5</v>
@@ -3933,7 +4214,7 @@
         <v>110</v>
       </c>
       <c r="F91" t="s">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="G91" t="s">
         <v>5</v>
@@ -3949,8 +4230,8 @@
       <c r="A92" t="s">
         <v>20</v>
       </c>
-      <c r="B92" t="s">
-        <v>20</v>
+      <c r="B92" s="2" t="s">
+        <v>366</v>
       </c>
       <c r="C92" t="s">
         <v>20</v>
@@ -3962,7 +4243,7 @@
         <v>111</v>
       </c>
       <c r="F92" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="G92" t="s">
         <v>271</v>
@@ -3991,7 +4272,7 @@
         <v>112</v>
       </c>
       <c r="F93" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="G93" t="s">
         <v>261</v>
@@ -4008,19 +4289,19 @@
         <v>20</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>308</v>
       </c>
       <c r="C94" t="s">
         <v>20</v>
       </c>
-      <c r="D94" t="s">
-        <v>20</v>
+      <c r="D94" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E94" t="s">
         <v>113</v>
       </c>
       <c r="F94" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="G94" t="s">
         <v>263</v>
@@ -4049,7 +4330,7 @@
         <v>114</v>
       </c>
       <c r="F95" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="G95" t="s">
         <v>261</v>
@@ -4078,7 +4359,7 @@
         <v>115</v>
       </c>
       <c r="F96" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="G96" t="s">
         <v>263</v>
@@ -4095,7 +4376,7 @@
         <v>20</v>
       </c>
       <c r="B97" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="C97" t="s">
         <v>20</v>
@@ -4107,7 +4388,7 @@
         <v>116</v>
       </c>
       <c r="F97" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="G97" t="s">
         <v>263</v>
@@ -4123,8 +4404,8 @@
       <c r="A98" t="s">
         <v>20</v>
       </c>
-      <c r="B98" t="s">
-        <v>20</v>
+      <c r="B98" s="2" t="s">
+        <v>367</v>
       </c>
       <c r="C98" t="s">
         <v>20</v>
@@ -4136,7 +4417,7 @@
         <v>117</v>
       </c>
       <c r="F98" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
       <c r="G98" t="s">
         <v>272</v>
@@ -4153,7 +4434,7 @@
         <v>20</v>
       </c>
       <c r="B99" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="C99" t="s">
         <v>20</v>
@@ -4165,7 +4446,7 @@
         <v>118</v>
       </c>
       <c r="F99" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
       <c r="G99" t="s">
         <v>263</v>
@@ -4182,7 +4463,7 @@
         <v>20</v>
       </c>
       <c r="B100" t="s">
-        <v>20</v>
+        <v>311</v>
       </c>
       <c r="C100" t="s">
         <v>20</v>
@@ -4194,7 +4475,7 @@
         <v>119</v>
       </c>
       <c r="F100" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="G100" t="s">
         <v>263</v>
@@ -4210,8 +4491,8 @@
       <c r="A101" t="s">
         <v>20</v>
       </c>
-      <c r="B101" t="s">
-        <v>20</v>
+      <c r="B101" s="2" t="s">
+        <v>368</v>
       </c>
       <c r="C101" t="s">
         <v>20</v>
@@ -4223,7 +4504,7 @@
         <v>120</v>
       </c>
       <c r="F101" t="s">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G101" t="s">
         <v>273</v>
@@ -4240,7 +4521,7 @@
         <v>20</v>
       </c>
       <c r="B102" t="s">
-        <v>20</v>
+        <v>312</v>
       </c>
       <c r="C102" t="s">
         <v>20</v>
@@ -4252,7 +4533,7 @@
         <v>121</v>
       </c>
       <c r="F102" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="G102" t="s">
         <v>263</v>
@@ -4269,7 +4550,7 @@
         <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>20</v>
+        <v>313</v>
       </c>
       <c r="C103" t="s">
         <v>20</v>
@@ -4281,7 +4562,7 @@
         <v>122</v>
       </c>
       <c r="F103" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="G103" t="s">
         <v>5</v>
@@ -4298,7 +4579,7 @@
         <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>20</v>
+        <v>314</v>
       </c>
       <c r="C104" t="s">
         <v>20</v>
@@ -4310,7 +4591,7 @@
         <v>123</v>
       </c>
       <c r="F104" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="G104" t="s">
         <v>5</v>
@@ -4327,7 +4608,7 @@
         <v>20</v>
       </c>
       <c r="B105" t="s">
-        <v>20</v>
+        <v>315</v>
       </c>
       <c r="C105" t="s">
         <v>20</v>
@@ -4339,7 +4620,7 @@
         <v>124</v>
       </c>
       <c r="F105" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="G105" t="s">
         <v>265</v>
@@ -4355,9 +4636,6 @@
       <c r="A106" t="s">
         <v>20</v>
       </c>
-      <c r="B106" t="s">
-        <v>20</v>
-      </c>
       <c r="C106" t="s">
         <v>20</v>
       </c>
@@ -4368,7 +4646,7 @@
         <v>125</v>
       </c>
       <c r="F106" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="G106" t="s">
         <v>5</v>
@@ -4397,7 +4675,7 @@
         <v>126</v>
       </c>
       <c r="F107" t="s">
-        <v>126</v>
+        <v>20</v>
       </c>
       <c r="G107" t="s">
         <v>5</v>
@@ -4426,7 +4704,7 @@
         <v>127</v>
       </c>
       <c r="F108" t="s">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="G108" t="s">
         <v>5</v>
@@ -4455,7 +4733,7 @@
         <v>128</v>
       </c>
       <c r="F109" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="G109" t="s">
         <v>5</v>
@@ -4484,7 +4762,7 @@
         <v>129</v>
       </c>
       <c r="F110" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="G110" t="s">
         <v>5</v>
@@ -4513,7 +4791,7 @@
         <v>130</v>
       </c>
       <c r="F111" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="G111" t="s">
         <v>5</v>
@@ -4542,7 +4820,7 @@
         <v>131</v>
       </c>
       <c r="F112" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="G112" t="s">
         <v>5</v>
@@ -4571,7 +4849,7 @@
         <v>132</v>
       </c>
       <c r="F113" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="G113" t="s">
         <v>5</v>
@@ -4587,8 +4865,8 @@
       <c r="A114" t="s">
         <v>20</v>
       </c>
-      <c r="B114" t="s">
-        <v>20</v>
+      <c r="B114" s="2" t="s">
+        <v>369</v>
       </c>
       <c r="C114" t="s">
         <v>20</v>
@@ -4600,7 +4878,7 @@
         <v>133</v>
       </c>
       <c r="F114" t="s">
-        <v>133</v>
+        <v>20</v>
       </c>
       <c r="G114" t="s">
         <v>274</v>
@@ -4617,7 +4895,7 @@
         <v>20</v>
       </c>
       <c r="B115" t="s">
-        <v>20</v>
+        <v>316</v>
       </c>
       <c r="C115" t="s">
         <v>20</v>
@@ -4629,7 +4907,7 @@
         <v>134</v>
       </c>
       <c r="F115" t="s">
-        <v>134</v>
+        <v>20</v>
       </c>
       <c r="G115" t="s">
         <v>263</v>
@@ -4646,7 +4924,7 @@
         <v>20</v>
       </c>
       <c r="B116" t="s">
-        <v>20</v>
+        <v>317</v>
       </c>
       <c r="C116" t="s">
         <v>20</v>
@@ -4658,7 +4936,7 @@
         <v>135</v>
       </c>
       <c r="F116" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="G116" t="s">
         <v>265</v>
@@ -4674,9 +4952,6 @@
       <c r="A117" t="s">
         <v>20</v>
       </c>
-      <c r="B117" t="s">
-        <v>20</v>
-      </c>
       <c r="C117" t="s">
         <v>20</v>
       </c>
@@ -4687,7 +4962,7 @@
         <v>136</v>
       </c>
       <c r="F117" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="G117" t="s">
         <v>5</v>
@@ -4716,7 +4991,7 @@
         <v>137</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>20</v>
       </c>
       <c r="G118" t="s">
         <v>5</v>
@@ -4745,7 +5020,7 @@
         <v>138</v>
       </c>
       <c r="F119" t="s">
-        <v>138</v>
+        <v>20</v>
       </c>
       <c r="G119" t="s">
         <v>5</v>
@@ -4774,7 +5049,7 @@
         <v>139</v>
       </c>
       <c r="F120" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="G120" t="s">
         <v>5</v>
@@ -4803,7 +5078,7 @@
         <v>140</v>
       </c>
       <c r="F121" t="s">
-        <v>140</v>
+        <v>20</v>
       </c>
       <c r="G121" t="s">
         <v>5</v>
@@ -4832,7 +5107,7 @@
         <v>141</v>
       </c>
       <c r="F122" t="s">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="G122" t="s">
         <v>5</v>
@@ -4861,7 +5136,7 @@
         <v>142</v>
       </c>
       <c r="F123" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="G123" t="s">
         <v>5</v>
@@ -4890,7 +5165,7 @@
         <v>143</v>
       </c>
       <c r="F124" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="G124" t="s">
         <v>5</v>
@@ -4906,9 +5181,7 @@
       <c r="A125" t="s">
         <v>20</v>
       </c>
-      <c r="B125" t="s">
-        <v>20</v>
-      </c>
+      <c r="B125" s="2"/>
       <c r="C125" t="s">
         <v>20</v>
       </c>
@@ -4919,7 +5192,7 @@
         <v>144</v>
       </c>
       <c r="F125" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="G125" t="s">
         <v>275</v>
@@ -4936,7 +5209,7 @@
         <v>20</v>
       </c>
       <c r="B126" t="s">
-        <v>20</v>
+        <v>318</v>
       </c>
       <c r="C126" t="s">
         <v>20</v>
@@ -4948,7 +5221,7 @@
         <v>145</v>
       </c>
       <c r="F126" t="s">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="G126" t="s">
         <v>263</v>
@@ -4965,7 +5238,7 @@
         <v>20</v>
       </c>
       <c r="B127" t="s">
-        <v>20</v>
+        <v>319</v>
       </c>
       <c r="C127" t="s">
         <v>20</v>
@@ -4977,7 +5250,7 @@
         <v>146</v>
       </c>
       <c r="F127" t="s">
-        <v>146</v>
+        <v>20</v>
       </c>
       <c r="G127" t="s">
         <v>276</v>
@@ -4994,7 +5267,7 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="C128" t="s">
         <v>20</v>
@@ -5006,7 +5279,7 @@
         <v>147</v>
       </c>
       <c r="F128" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="G128" t="s">
         <v>263</v>
@@ -5035,7 +5308,7 @@
         <v>148</v>
       </c>
       <c r="F129" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
       <c r="G129" t="s">
         <v>261</v>
@@ -5052,7 +5325,7 @@
         <v>20</v>
       </c>
       <c r="B130" t="s">
-        <v>20</v>
+        <v>321</v>
       </c>
       <c r="C130" t="s">
         <v>20</v>
@@ -5064,7 +5337,7 @@
         <v>149</v>
       </c>
       <c r="F130" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G130" t="s">
         <v>263</v>
@@ -5093,7 +5366,7 @@
         <v>150</v>
       </c>
       <c r="F131" t="s">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="G131" t="s">
         <v>261</v>
@@ -5110,7 +5383,7 @@
         <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>20</v>
+        <v>322</v>
       </c>
       <c r="C132" t="s">
         <v>20</v>
@@ -5122,7 +5395,7 @@
         <v>151</v>
       </c>
       <c r="F132" t="s">
-        <v>151</v>
+        <v>20</v>
       </c>
       <c r="G132" t="s">
         <v>263</v>
@@ -5139,7 +5412,7 @@
         <v>20</v>
       </c>
       <c r="B133" t="s">
-        <v>20</v>
+        <v>323</v>
       </c>
       <c r="C133" t="s">
         <v>20</v>
@@ -5151,7 +5424,7 @@
         <v>152</v>
       </c>
       <c r="F133" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="G133" t="s">
         <v>263</v>
@@ -5180,7 +5453,7 @@
         <v>153</v>
       </c>
       <c r="F134" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="G134" t="s">
         <v>261</v>
@@ -5209,7 +5482,7 @@
         <v>154</v>
       </c>
       <c r="F135" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="G135" t="s">
         <v>263</v>
@@ -5238,7 +5511,7 @@
         <v>155</v>
       </c>
       <c r="F136" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="G136" t="s">
         <v>261</v>
@@ -5267,7 +5540,7 @@
         <v>156</v>
       </c>
       <c r="F137" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="G137" t="s">
         <v>263</v>
@@ -5284,7 +5557,7 @@
         <v>20</v>
       </c>
       <c r="B138" t="s">
-        <v>20</v>
+        <v>324</v>
       </c>
       <c r="C138" t="s">
         <v>20</v>
@@ -5296,7 +5569,7 @@
         <v>157</v>
       </c>
       <c r="F138" t="s">
-        <v>157</v>
+        <v>20</v>
       </c>
       <c r="G138" t="s">
         <v>263</v>
@@ -5313,7 +5586,7 @@
         <v>20</v>
       </c>
       <c r="B139" t="s">
-        <v>20</v>
+        <v>325</v>
       </c>
       <c r="C139" t="s">
         <v>20</v>
@@ -5325,7 +5598,7 @@
         <v>158</v>
       </c>
       <c r="F139" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
       <c r="G139" t="s">
         <v>263</v>
@@ -5342,7 +5615,7 @@
         <v>20</v>
       </c>
       <c r="B140" t="s">
-        <v>20</v>
+        <v>298</v>
       </c>
       <c r="C140" t="s">
         <v>20</v>
@@ -5354,7 +5627,7 @@
         <v>159</v>
       </c>
       <c r="F140" t="s">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="G140" t="s">
         <v>277</v>
@@ -5371,19 +5644,19 @@
         <v>20</v>
       </c>
       <c r="B141" t="s">
-        <v>20</v>
+        <v>326</v>
       </c>
       <c r="C141" t="s">
         <v>20</v>
       </c>
-      <c r="D141" t="s">
-        <v>20</v>
+      <c r="D141" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E141" t="s">
         <v>160</v>
       </c>
       <c r="F141" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="G141" t="s">
         <v>5</v>
@@ -5400,7 +5673,7 @@
         <v>20</v>
       </c>
       <c r="B142" t="s">
-        <v>20</v>
+        <v>327</v>
       </c>
       <c r="C142" t="s">
         <v>20</v>
@@ -5412,7 +5685,7 @@
         <v>161</v>
       </c>
       <c r="F142" t="s">
-        <v>161</v>
+        <v>20</v>
       </c>
       <c r="G142" t="s">
         <v>265</v>
@@ -5428,9 +5701,6 @@
       <c r="A143" t="s">
         <v>20</v>
       </c>
-      <c r="B143" t="s">
-        <v>20</v>
-      </c>
       <c r="C143" t="s">
         <v>20</v>
       </c>
@@ -5441,7 +5711,7 @@
         <v>162</v>
       </c>
       <c r="F143" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="G143" t="s">
         <v>5</v>
@@ -5470,7 +5740,7 @@
         <v>163</v>
       </c>
       <c r="F144" t="s">
-        <v>163</v>
+        <v>20</v>
       </c>
       <c r="G144" t="s">
         <v>5</v>
@@ -5499,7 +5769,7 @@
         <v>164</v>
       </c>
       <c r="F145" t="s">
-        <v>164</v>
+        <v>20</v>
       </c>
       <c r="G145" t="s">
         <v>5</v>
@@ -5528,7 +5798,7 @@
         <v>165</v>
       </c>
       <c r="F146" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="G146" t="s">
         <v>5</v>
@@ -5557,7 +5827,7 @@
         <v>166</v>
       </c>
       <c r="F147" t="s">
-        <v>166</v>
+        <v>20</v>
       </c>
       <c r="G147" t="s">
         <v>5</v>
@@ -5586,7 +5856,7 @@
         <v>167</v>
       </c>
       <c r="F148" t="s">
-        <v>167</v>
+        <v>20</v>
       </c>
       <c r="G148" t="s">
         <v>5</v>
@@ -5615,7 +5885,7 @@
         <v>168</v>
       </c>
       <c r="F149" t="s">
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G149" t="s">
         <v>5</v>
@@ -5631,8 +5901,8 @@
       <c r="A150" t="s">
         <v>20</v>
       </c>
-      <c r="B150" t="s">
-        <v>20</v>
+      <c r="B150" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="C150" t="s">
         <v>20</v>
@@ -5644,7 +5914,7 @@
         <v>169</v>
       </c>
       <c r="F150" t="s">
-        <v>169</v>
+        <v>20</v>
       </c>
       <c r="G150" t="s">
         <v>278</v>
@@ -5660,20 +5930,20 @@
       <c r="A151" t="s">
         <v>20</v>
       </c>
-      <c r="B151" t="s">
-        <v>20</v>
+      <c r="B151" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="C151" t="s">
         <v>20</v>
       </c>
-      <c r="D151" t="s">
-        <v>20</v>
+      <c r="D151" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E151" t="s">
         <v>170</v>
       </c>
       <c r="F151" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="G151" t="s">
         <v>5</v>
@@ -5702,7 +5972,7 @@
         <v>171</v>
       </c>
       <c r="F152" t="s">
-        <v>171</v>
+        <v>20</v>
       </c>
       <c r="G152" t="s">
         <v>261</v>
@@ -5719,7 +5989,7 @@
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>20</v>
+        <v>328</v>
       </c>
       <c r="C153" t="s">
         <v>20</v>
@@ -5731,7 +6001,7 @@
         <v>172</v>
       </c>
       <c r="F153" t="s">
-        <v>172</v>
+        <v>20</v>
       </c>
       <c r="G153" t="s">
         <v>279</v>
@@ -5747,9 +6017,6 @@
       <c r="A154" t="s">
         <v>20</v>
       </c>
-      <c r="B154" t="s">
-        <v>20</v>
-      </c>
       <c r="C154" t="s">
         <v>20</v>
       </c>
@@ -5760,7 +6027,7 @@
         <v>173</v>
       </c>
       <c r="F154" t="s">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="G154" t="s">
         <v>5</v>
@@ -5789,7 +6056,7 @@
         <v>174</v>
       </c>
       <c r="F155" t="s">
-        <v>174</v>
+        <v>20</v>
       </c>
       <c r="G155" t="s">
         <v>5</v>
@@ -5818,7 +6085,7 @@
         <v>175</v>
       </c>
       <c r="F156" t="s">
-        <v>175</v>
+        <v>20</v>
       </c>
       <c r="G156" t="s">
         <v>5</v>
@@ -5847,7 +6114,7 @@
         <v>176</v>
       </c>
       <c r="F157" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="G157" t="s">
         <v>5</v>
@@ -5876,7 +6143,7 @@
         <v>177</v>
       </c>
       <c r="F158" t="s">
-        <v>177</v>
+        <v>20</v>
       </c>
       <c r="G158" t="s">
         <v>5</v>
@@ -5905,7 +6172,7 @@
         <v>178</v>
       </c>
       <c r="F159" t="s">
-        <v>178</v>
+        <v>20</v>
       </c>
       <c r="G159" t="s">
         <v>5</v>
@@ -5934,7 +6201,7 @@
         <v>179</v>
       </c>
       <c r="F160" t="s">
-        <v>179</v>
+        <v>20</v>
       </c>
       <c r="G160" t="s">
         <v>5</v>
@@ -5963,7 +6230,7 @@
         <v>180</v>
       </c>
       <c r="F161" t="s">
-        <v>180</v>
+        <v>20</v>
       </c>
       <c r="G161" t="s">
         <v>5</v>
@@ -5992,7 +6259,7 @@
         <v>181</v>
       </c>
       <c r="F162" t="s">
-        <v>181</v>
+        <v>20</v>
       </c>
       <c r="G162" t="s">
         <v>5</v>
@@ -6021,7 +6288,7 @@
         <v>182</v>
       </c>
       <c r="F163" t="s">
-        <v>182</v>
+        <v>20</v>
       </c>
       <c r="G163" t="s">
         <v>5</v>
@@ -6050,7 +6317,7 @@
         <v>183</v>
       </c>
       <c r="F164" t="s">
-        <v>183</v>
+        <v>20</v>
       </c>
       <c r="G164" t="s">
         <v>261</v>
@@ -6079,7 +6346,7 @@
         <v>184</v>
       </c>
       <c r="F165" t="s">
-        <v>184</v>
+        <v>20</v>
       </c>
       <c r="G165" t="s">
         <v>263</v>
@@ -6095,8 +6362,8 @@
       <c r="A166" t="s">
         <v>20</v>
       </c>
-      <c r="B166" t="s">
-        <v>20</v>
+      <c r="B166" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="C166" t="s">
         <v>20</v>
@@ -6108,7 +6375,7 @@
         <v>185</v>
       </c>
       <c r="F166" t="s">
-        <v>185</v>
+        <v>20</v>
       </c>
       <c r="G166" t="s">
         <v>280</v>
@@ -6137,7 +6404,7 @@
         <v>186</v>
       </c>
       <c r="F167" t="s">
-        <v>186</v>
+        <v>20</v>
       </c>
       <c r="G167" t="s">
         <v>261</v>
@@ -6154,7 +6421,7 @@
         <v>20</v>
       </c>
       <c r="B168" t="s">
-        <v>20</v>
+        <v>329</v>
       </c>
       <c r="C168" t="s">
         <v>20</v>
@@ -6166,7 +6433,7 @@
         <v>187</v>
       </c>
       <c r="F168" t="s">
-        <v>187</v>
+        <v>20</v>
       </c>
       <c r="G168" t="s">
         <v>5</v>
@@ -6183,7 +6450,7 @@
         <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>20</v>
+        <v>330</v>
       </c>
       <c r="C169" t="s">
         <v>20</v>
@@ -6195,7 +6462,7 @@
         <v>188</v>
       </c>
       <c r="F169" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="G169" t="s">
         <v>263</v>
@@ -6212,7 +6479,7 @@
         <v>20</v>
       </c>
       <c r="B170" t="s">
-        <v>20</v>
+        <v>331</v>
       </c>
       <c r="C170" t="s">
         <v>20</v>
@@ -6224,7 +6491,7 @@
         <v>189</v>
       </c>
       <c r="F170" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="G170" t="s">
         <v>5</v>
@@ -6253,7 +6520,7 @@
         <v>190</v>
       </c>
       <c r="F171" t="s">
-        <v>190</v>
+        <v>20</v>
       </c>
       <c r="G171" t="s">
         <v>261</v>
@@ -6282,7 +6549,7 @@
         <v>191</v>
       </c>
       <c r="F172" t="s">
-        <v>191</v>
+        <v>20</v>
       </c>
       <c r="G172" t="s">
         <v>263</v>
@@ -6299,7 +6566,7 @@
         <v>20</v>
       </c>
       <c r="B173" t="s">
-        <v>20</v>
+        <v>332</v>
       </c>
       <c r="C173" t="s">
         <v>20</v>
@@ -6311,7 +6578,7 @@
         <v>192</v>
       </c>
       <c r="F173" t="s">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="G173" t="s">
         <v>281</v>
@@ -6340,7 +6607,7 @@
         <v>193</v>
       </c>
       <c r="F174" t="s">
-        <v>193</v>
+        <v>20</v>
       </c>
       <c r="G174" t="s">
         <v>261</v>
@@ -6357,7 +6624,7 @@
         <v>20</v>
       </c>
       <c r="B175" t="s">
-        <v>20</v>
+        <v>333</v>
       </c>
       <c r="C175" t="s">
         <v>20</v>
@@ -6369,7 +6636,7 @@
         <v>194</v>
       </c>
       <c r="F175" t="s">
-        <v>194</v>
+        <v>20</v>
       </c>
       <c r="G175" t="s">
         <v>263</v>
@@ -6386,7 +6653,7 @@
         <v>20</v>
       </c>
       <c r="B176" t="s">
-        <v>20</v>
+        <v>334</v>
       </c>
       <c r="C176" t="s">
         <v>20</v>
@@ -6398,7 +6665,7 @@
         <v>195</v>
       </c>
       <c r="F176" t="s">
-        <v>195</v>
+        <v>20</v>
       </c>
       <c r="G176" t="s">
         <v>263</v>
@@ -6415,7 +6682,7 @@
         <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>20</v>
+        <v>335</v>
       </c>
       <c r="C177" t="s">
         <v>20</v>
@@ -6427,7 +6694,7 @@
         <v>196</v>
       </c>
       <c r="F177" t="s">
-        <v>196</v>
+        <v>20</v>
       </c>
       <c r="G177" t="s">
         <v>263</v>
@@ -6456,7 +6723,7 @@
         <v>197</v>
       </c>
       <c r="F178" t="s">
-        <v>197</v>
+        <v>20</v>
       </c>
       <c r="G178" t="s">
         <v>261</v>
@@ -6485,7 +6752,7 @@
         <v>198</v>
       </c>
       <c r="F179" t="s">
-        <v>198</v>
+        <v>20</v>
       </c>
       <c r="G179" t="s">
         <v>263</v>
@@ -6502,7 +6769,7 @@
         <v>20</v>
       </c>
       <c r="B180" t="s">
-        <v>20</v>
+        <v>336</v>
       </c>
       <c r="C180" t="s">
         <v>20</v>
@@ -6514,7 +6781,7 @@
         <v>199</v>
       </c>
       <c r="F180" t="s">
-        <v>199</v>
+        <v>20</v>
       </c>
       <c r="G180" t="s">
         <v>263</v>
@@ -6543,7 +6810,7 @@
         <v>200</v>
       </c>
       <c r="F181" t="s">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="G181" t="s">
         <v>261</v>
@@ -6560,7 +6827,7 @@
         <v>20</v>
       </c>
       <c r="B182" t="s">
-        <v>20</v>
+        <v>337</v>
       </c>
       <c r="C182" t="s">
         <v>20</v>
@@ -6572,7 +6839,7 @@
         <v>201</v>
       </c>
       <c r="F182" t="s">
-        <v>201</v>
+        <v>20</v>
       </c>
       <c r="G182" t="s">
         <v>5</v>
@@ -6589,7 +6856,7 @@
         <v>20</v>
       </c>
       <c r="B183" t="s">
-        <v>20</v>
+        <v>338</v>
       </c>
       <c r="C183" t="s">
         <v>20</v>
@@ -6601,7 +6868,7 @@
         <v>202</v>
       </c>
       <c r="F183" t="s">
-        <v>202</v>
+        <v>20</v>
       </c>
       <c r="G183" t="s">
         <v>263</v>
@@ -6630,7 +6897,7 @@
         <v>203</v>
       </c>
       <c r="F184" t="s">
-        <v>203</v>
+        <v>20</v>
       </c>
       <c r="G184" t="s">
         <v>261</v>
@@ -6659,7 +6926,7 @@
         <v>204</v>
       </c>
       <c r="F185" t="s">
-        <v>204</v>
+        <v>20</v>
       </c>
       <c r="G185" t="s">
         <v>263</v>
@@ -6676,7 +6943,7 @@
         <v>20</v>
       </c>
       <c r="B186" t="s">
-        <v>20</v>
+        <v>339</v>
       </c>
       <c r="C186" t="s">
         <v>20</v>
@@ -6688,7 +6955,7 @@
         <v>205</v>
       </c>
       <c r="F186" t="s">
-        <v>205</v>
+        <v>20</v>
       </c>
       <c r="G186" t="s">
         <v>263</v>
@@ -6717,7 +6984,7 @@
         <v>206</v>
       </c>
       <c r="F187" t="s">
-        <v>206</v>
+        <v>20</v>
       </c>
       <c r="G187" t="s">
         <v>261</v>
@@ -6734,7 +7001,7 @@
         <v>20</v>
       </c>
       <c r="B188" t="s">
-        <v>20</v>
+        <v>340</v>
       </c>
       <c r="C188" t="s">
         <v>20</v>
@@ -6746,7 +7013,7 @@
         <v>207</v>
       </c>
       <c r="F188" t="s">
-        <v>207</v>
+        <v>20</v>
       </c>
       <c r="G188" t="s">
         <v>263</v>
@@ -6775,7 +7042,7 @@
         <v>208</v>
       </c>
       <c r="F189" t="s">
-        <v>208</v>
+        <v>20</v>
       </c>
       <c r="G189" t="s">
         <v>261</v>
@@ -6804,7 +7071,7 @@
         <v>209</v>
       </c>
       <c r="F190" t="s">
-        <v>209</v>
+        <v>20</v>
       </c>
       <c r="G190" t="s">
         <v>263</v>
@@ -6821,7 +7088,7 @@
         <v>20</v>
       </c>
       <c r="B191" t="s">
-        <v>20</v>
+        <v>341</v>
       </c>
       <c r="C191" t="s">
         <v>20</v>
@@ -6833,7 +7100,7 @@
         <v>210</v>
       </c>
       <c r="F191" t="s">
-        <v>210</v>
+        <v>20</v>
       </c>
       <c r="G191" t="s">
         <v>263</v>
@@ -6850,7 +7117,7 @@
         <v>20</v>
       </c>
       <c r="B192" t="s">
-        <v>20</v>
+        <v>342</v>
       </c>
       <c r="C192" t="s">
         <v>20</v>
@@ -6862,7 +7129,7 @@
         <v>211</v>
       </c>
       <c r="F192" t="s">
-        <v>211</v>
+        <v>20</v>
       </c>
       <c r="G192" t="s">
         <v>263</v>
@@ -6891,7 +7158,7 @@
         <v>212</v>
       </c>
       <c r="F193" t="s">
-        <v>212</v>
+        <v>20</v>
       </c>
       <c r="G193" t="s">
         <v>261</v>
@@ -6908,7 +7175,7 @@
         <v>20</v>
       </c>
       <c r="B194" t="s">
-        <v>20</v>
+        <v>343</v>
       </c>
       <c r="C194" t="s">
         <v>20</v>
@@ -6920,7 +7187,7 @@
         <v>213</v>
       </c>
       <c r="F194" t="s">
-        <v>213</v>
+        <v>20</v>
       </c>
       <c r="G194" t="s">
         <v>263</v>
@@ -6949,7 +7216,7 @@
         <v>214</v>
       </c>
       <c r="F195" t="s">
-        <v>214</v>
+        <v>20</v>
       </c>
       <c r="G195" t="s">
         <v>261</v>
@@ -6978,7 +7245,7 @@
         <v>215</v>
       </c>
       <c r="F196" t="s">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="G196" t="s">
         <v>263</v>
@@ -7007,7 +7274,7 @@
         <v>216</v>
       </c>
       <c r="F197" t="s">
-        <v>216</v>
+        <v>20</v>
       </c>
       <c r="G197" t="s">
         <v>261</v>
@@ -7024,19 +7291,19 @@
         <v>20</v>
       </c>
       <c r="B198" t="s">
-        <v>20</v>
+        <v>344</v>
       </c>
       <c r="C198" t="s">
         <v>20</v>
       </c>
-      <c r="D198" t="s">
-        <v>20</v>
+      <c r="D198" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E198" t="s">
         <v>217</v>
       </c>
       <c r="F198" t="s">
-        <v>217</v>
+        <v>20</v>
       </c>
       <c r="G198" t="s">
         <v>263</v>
@@ -7065,7 +7332,7 @@
         <v>218</v>
       </c>
       <c r="F199" t="s">
-        <v>218</v>
+        <v>20</v>
       </c>
       <c r="G199" t="s">
         <v>261</v>
@@ -7094,7 +7361,7 @@
         <v>219</v>
       </c>
       <c r="F200" t="s">
-        <v>219</v>
+        <v>20</v>
       </c>
       <c r="G200" t="s">
         <v>263</v>
@@ -7111,19 +7378,19 @@
         <v>20</v>
       </c>
       <c r="B201" t="s">
-        <v>20</v>
+        <v>345</v>
       </c>
       <c r="C201" t="s">
         <v>20</v>
       </c>
-      <c r="D201" t="s">
-        <v>20</v>
+      <c r="D201" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E201" t="s">
         <v>220</v>
       </c>
       <c r="F201" t="s">
-        <v>220</v>
+        <v>20</v>
       </c>
       <c r="G201" t="s">
         <v>263</v>
@@ -7140,7 +7407,7 @@
         <v>20</v>
       </c>
       <c r="B202" t="s">
-        <v>20</v>
+        <v>346</v>
       </c>
       <c r="C202" t="s">
         <v>20</v>
@@ -7152,7 +7419,7 @@
         <v>221</v>
       </c>
       <c r="F202" t="s">
-        <v>221</v>
+        <v>20</v>
       </c>
       <c r="G202" t="s">
         <v>263</v>
@@ -7168,8 +7435,8 @@
       <c r="A203" t="s">
         <v>20</v>
       </c>
-      <c r="B203" t="s">
-        <v>20</v>
+      <c r="B203" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="C203" t="s">
         <v>20</v>
@@ -7181,7 +7448,7 @@
         <v>222</v>
       </c>
       <c r="F203" t="s">
-        <v>222</v>
+        <v>20</v>
       </c>
       <c r="G203" t="s">
         <v>282</v>
@@ -7210,7 +7477,7 @@
         <v>223</v>
       </c>
       <c r="F204" t="s">
-        <v>223</v>
+        <v>20</v>
       </c>
       <c r="G204" t="s">
         <v>261</v>
@@ -7227,7 +7494,7 @@
         <v>20</v>
       </c>
       <c r="B205" t="s">
-        <v>20</v>
+        <v>347</v>
       </c>
       <c r="C205" t="s">
         <v>20</v>
@@ -7239,7 +7506,7 @@
         <v>224</v>
       </c>
       <c r="F205" t="s">
-        <v>224</v>
+        <v>20</v>
       </c>
       <c r="G205" t="s">
         <v>5</v>
@@ -7268,7 +7535,7 @@
         <v>225</v>
       </c>
       <c r="F206" t="s">
-        <v>225</v>
+        <v>20</v>
       </c>
       <c r="G206" t="s">
         <v>261</v>
@@ -7297,7 +7564,7 @@
         <v>226</v>
       </c>
       <c r="F207" t="s">
-        <v>226</v>
+        <v>20</v>
       </c>
       <c r="G207" t="s">
         <v>263</v>
@@ -7314,7 +7581,7 @@
         <v>20</v>
       </c>
       <c r="B208" t="s">
-        <v>20</v>
+        <v>348</v>
       </c>
       <c r="C208" t="s">
         <v>20</v>
@@ -7326,7 +7593,7 @@
         <v>227</v>
       </c>
       <c r="F208" t="s">
-        <v>227</v>
+        <v>20</v>
       </c>
       <c r="G208" t="s">
         <v>263</v>
@@ -7355,7 +7622,7 @@
         <v>228</v>
       </c>
       <c r="F209" t="s">
-        <v>228</v>
+        <v>20</v>
       </c>
       <c r="G209" t="s">
         <v>261</v>
@@ -7372,7 +7639,7 @@
         <v>20</v>
       </c>
       <c r="B210" t="s">
-        <v>20</v>
+        <v>349</v>
       </c>
       <c r="C210" t="s">
         <v>20</v>
@@ -7384,7 +7651,7 @@
         <v>229</v>
       </c>
       <c r="F210" t="s">
-        <v>229</v>
+        <v>20</v>
       </c>
       <c r="G210" t="s">
         <v>263</v>
@@ -7413,7 +7680,7 @@
         <v>230</v>
       </c>
       <c r="F211" t="s">
-        <v>230</v>
+        <v>20</v>
       </c>
       <c r="G211" t="s">
         <v>261</v>
@@ -7442,7 +7709,7 @@
         <v>231</v>
       </c>
       <c r="F212" t="s">
-        <v>231</v>
+        <v>20</v>
       </c>
       <c r="G212" t="s">
         <v>263</v>
@@ -7459,7 +7726,7 @@
         <v>20</v>
       </c>
       <c r="B213" t="s">
-        <v>20</v>
+        <v>350</v>
       </c>
       <c r="C213" t="s">
         <v>20</v>
@@ -7471,7 +7738,7 @@
         <v>232</v>
       </c>
       <c r="F213" t="s">
-        <v>232</v>
+        <v>20</v>
       </c>
       <c r="G213" t="s">
         <v>283</v>
@@ -7488,7 +7755,7 @@
         <v>20</v>
       </c>
       <c r="B214" t="s">
-        <v>20</v>
+        <v>351</v>
       </c>
       <c r="C214" t="s">
         <v>20</v>
@@ -7500,7 +7767,7 @@
         <v>233</v>
       </c>
       <c r="F214" t="s">
-        <v>233</v>
+        <v>20</v>
       </c>
       <c r="G214" t="s">
         <v>5</v>
@@ -7517,7 +7784,7 @@
         <v>20</v>
       </c>
       <c r="B215" t="s">
-        <v>20</v>
+        <v>352</v>
       </c>
       <c r="C215" t="s">
         <v>20</v>
@@ -7529,7 +7796,7 @@
         <v>234</v>
       </c>
       <c r="F215" t="s">
-        <v>234</v>
+        <v>20</v>
       </c>
       <c r="G215" t="s">
         <v>5</v>
@@ -7546,7 +7813,7 @@
         <v>20</v>
       </c>
       <c r="B216" t="s">
-        <v>20</v>
+        <v>353</v>
       </c>
       <c r="C216" t="s">
         <v>20</v>
@@ -7558,7 +7825,7 @@
         <v>235</v>
       </c>
       <c r="F216" t="s">
-        <v>235</v>
+        <v>20</v>
       </c>
       <c r="G216" t="s">
         <v>263</v>
@@ -7575,7 +7842,7 @@
         <v>20</v>
       </c>
       <c r="B217" t="s">
-        <v>20</v>
+        <v>354</v>
       </c>
       <c r="C217" t="s">
         <v>20</v>
@@ -7587,7 +7854,7 @@
         <v>236</v>
       </c>
       <c r="F217" t="s">
-        <v>236</v>
+        <v>20</v>
       </c>
       <c r="G217" t="s">
         <v>5</v>
@@ -7604,7 +7871,7 @@
         <v>20</v>
       </c>
       <c r="B218" t="s">
-        <v>20</v>
+        <v>355</v>
       </c>
       <c r="C218" t="s">
         <v>20</v>
@@ -7616,7 +7883,7 @@
         <v>237</v>
       </c>
       <c r="F218" t="s">
-        <v>237</v>
+        <v>20</v>
       </c>
       <c r="G218" t="s">
         <v>263</v>
@@ -7633,7 +7900,7 @@
         <v>20</v>
       </c>
       <c r="B219" t="s">
-        <v>20</v>
+        <v>356</v>
       </c>
       <c r="C219" t="s">
         <v>20</v>
@@ -7645,7 +7912,7 @@
         <v>238</v>
       </c>
       <c r="F219" t="s">
-        <v>238</v>
+        <v>20</v>
       </c>
       <c r="G219" t="s">
         <v>5</v>
@@ -7662,19 +7929,19 @@
         <v>20</v>
       </c>
       <c r="B220" t="s">
-        <v>20</v>
+        <v>357</v>
       </c>
       <c r="C220" t="s">
         <v>20</v>
       </c>
-      <c r="D220" t="s">
-        <v>20</v>
+      <c r="D220" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E220" t="s">
         <v>239</v>
       </c>
       <c r="F220" t="s">
-        <v>239</v>
+        <v>20</v>
       </c>
       <c r="G220" t="s">
         <v>5</v>
@@ -7691,7 +7958,7 @@
         <v>20</v>
       </c>
       <c r="B221" t="s">
-        <v>20</v>
+        <v>358</v>
       </c>
       <c r="C221" t="s">
         <v>20</v>
@@ -7703,7 +7970,7 @@
         <v>240</v>
       </c>
       <c r="F221" t="s">
-        <v>240</v>
+        <v>20</v>
       </c>
       <c r="G221" t="s">
         <v>284</v>
@@ -7720,19 +7987,19 @@
         <v>20</v>
       </c>
       <c r="B222" t="s">
-        <v>20</v>
+        <v>359</v>
       </c>
       <c r="C222" t="s">
         <v>20</v>
       </c>
-      <c r="D222" t="s">
-        <v>20</v>
+      <c r="D222" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E222" t="s">
         <v>241</v>
       </c>
       <c r="F222" t="s">
-        <v>241</v>
+        <v>20</v>
       </c>
       <c r="G222" t="s">
         <v>5</v>
@@ -7749,7 +8016,7 @@
         <v>20</v>
       </c>
       <c r="B223" t="s">
-        <v>20</v>
+        <v>360</v>
       </c>
       <c r="C223" t="s">
         <v>20</v>
@@ -7761,7 +8028,7 @@
         <v>242</v>
       </c>
       <c r="F223" t="s">
-        <v>242</v>
+        <v>20</v>
       </c>
       <c r="G223" t="s">
         <v>285</v>
@@ -7777,9 +8044,6 @@
       <c r="A224" t="s">
         <v>20</v>
       </c>
-      <c r="B224" t="s">
-        <v>20</v>
-      </c>
       <c r="C224" t="s">
         <v>20</v>
       </c>
@@ -7790,7 +8054,7 @@
         <v>243</v>
       </c>
       <c r="F224" t="s">
-        <v>243</v>
+        <v>20</v>
       </c>
       <c r="G224" t="s">
         <v>5</v>
@@ -7819,7 +8083,7 @@
         <v>244</v>
       </c>
       <c r="F225" t="s">
-        <v>244</v>
+        <v>20</v>
       </c>
       <c r="G225" t="s">
         <v>5</v>
@@ -7848,7 +8112,7 @@
         <v>245</v>
       </c>
       <c r="F226" t="s">
-        <v>245</v>
+        <v>20</v>
       </c>
       <c r="G226" t="s">
         <v>5</v>
@@ -7877,7 +8141,7 @@
         <v>246</v>
       </c>
       <c r="F227" t="s">
-        <v>246</v>
+        <v>20</v>
       </c>
       <c r="G227" t="s">
         <v>5</v>
@@ -7906,7 +8170,7 @@
         <v>247</v>
       </c>
       <c r="F228" t="s">
-        <v>247</v>
+        <v>20</v>
       </c>
       <c r="G228" t="s">
         <v>5</v>
@@ -7935,7 +8199,7 @@
         <v>248</v>
       </c>
       <c r="F229" t="s">
-        <v>248</v>
+        <v>20</v>
       </c>
       <c r="G229" t="s">
         <v>5</v>
@@ -7964,7 +8228,7 @@
         <v>249</v>
       </c>
       <c r="F230" t="s">
-        <v>249</v>
+        <v>20</v>
       </c>
       <c r="G230" t="s">
         <v>5</v>
@@ -7993,7 +8257,7 @@
         <v>250</v>
       </c>
       <c r="F231" t="s">
-        <v>250</v>
+        <v>20</v>
       </c>
       <c r="G231" t="s">
         <v>5</v>
@@ -8009,8 +8273,8 @@
       <c r="A232" t="s">
         <v>20</v>
       </c>
-      <c r="B232" t="s">
-        <v>20</v>
+      <c r="B232" s="2" t="s">
+        <v>374</v>
       </c>
       <c r="C232" t="s">
         <v>20</v>
@@ -8022,7 +8286,7 @@
         <v>251</v>
       </c>
       <c r="F232" t="s">
-        <v>251</v>
+        <v>20</v>
       </c>
       <c r="G232" t="s">
         <v>286</v>
@@ -8039,7 +8303,7 @@
         <v>20</v>
       </c>
       <c r="B233" t="s">
-        <v>20</v>
+        <v>361</v>
       </c>
       <c r="C233" t="s">
         <v>20</v>
@@ -8051,7 +8315,7 @@
         <v>252</v>
       </c>
       <c r="F233" t="s">
-        <v>252</v>
+        <v>20</v>
       </c>
       <c r="G233" t="s">
         <v>5</v>
@@ -8080,7 +8344,7 @@
         <v>253</v>
       </c>
       <c r="F234" t="s">
-        <v>253</v>
+        <v>20</v>
       </c>
       <c r="G234" t="s">
         <v>263</v>
@@ -8109,7 +8373,7 @@
         <v>254</v>
       </c>
       <c r="F235" t="s">
-        <v>254</v>
+        <v>20</v>
       </c>
       <c r="G235" t="s">
         <v>260</v>
@@ -8126,7 +8390,7 @@
         <v>20</v>
       </c>
       <c r="B236" t="s">
-        <v>20</v>
+        <v>362</v>
       </c>
       <c r="C236" t="s">
         <v>20</v>
@@ -8138,7 +8402,7 @@
         <v>255</v>
       </c>
       <c r="F236" t="s">
-        <v>255</v>
+        <v>20</v>
       </c>
       <c r="G236" t="s">
         <v>287</v>
@@ -8167,7 +8431,7 @@
         <v>256</v>
       </c>
       <c r="F237" t="s">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="G237" t="s">
         <v>5</v>
@@ -8183,8 +8447,8 @@
       <c r="A238" t="s">
         <v>20</v>
       </c>
-      <c r="B238" t="s">
-        <v>20</v>
+      <c r="B238" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="C238" t="s">
         <v>20</v>
@@ -8196,7 +8460,7 @@
         <v>257</v>
       </c>
       <c r="F238" t="s">
-        <v>257</v>
+        <v>20</v>
       </c>
       <c r="G238" t="s">
         <v>5</v>
@@ -8209,6 +8473,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I238" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -8218,7 +8483,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cleaning and processing done
</commit_message>
<xml_diff>
--- a/Documentation/variables_codebook.xlsx
+++ b/Documentation/variables_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\Github\World Bank\Devolve\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BB8E95-61A1-4D70-8E2F-9BE6E0B76F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021B981B-EF51-4BB8-872D-8BBC34EDF963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="385">
   <si>
     <t>name</t>
   </si>
@@ -1132,9 +1132,6 @@
     <t>Other response to the DEV04 question</t>
   </si>
   <si>
-    <t>Question about all the requirements to participate in the Devolve-ICMS program</t>
-  </si>
-  <si>
     <t>Other response to the DEV08 question</t>
   </si>
   <si>
@@ -1193,6 +1190,9 @@
   </si>
   <si>
     <t>If the person is the adult responsible for the decisions in the household or if they could call the responsible</t>
+  </si>
+  <si>
+    <t>Awareness about the requirements to participate in the Devolve-ICMS program</t>
   </si>
 </sst>
 </file>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2006,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -2093,7 +2093,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -2122,7 +2122,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -2238,7 +2238,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -2383,7 +2383,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
@@ -2412,7 +2412,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -2470,7 +2470,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
@@ -2557,7 +2557,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
@@ -2642,7 +2642,7 @@
         <v>20</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C37" t="s">
         <v>20</v>
@@ -3048,7 +3048,7 @@
         <v>20</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -3309,7 +3309,7 @@
         <v>20</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C60" t="s">
         <v>20</v>
@@ -4231,7 +4231,7 @@
         <v>20</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C92" t="s">
         <v>20</v>
@@ -4405,7 +4405,7 @@
         <v>20</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C98" t="s">
         <v>20</v>
@@ -4492,7 +4492,7 @@
         <v>20</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C101" t="s">
         <v>20</v>
@@ -4866,7 +4866,7 @@
         <v>20</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C114" t="s">
         <v>20</v>
@@ -5902,7 +5902,7 @@
         <v>20</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C150" t="s">
         <v>20</v>
@@ -5931,7 +5931,7 @@
         <v>20</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C151" t="s">
         <v>20</v>
@@ -6363,7 +6363,7 @@
         <v>20</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C166" t="s">
         <v>20</v>
@@ -7436,7 +7436,7 @@
         <v>20</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C203" t="s">
         <v>20</v>
@@ -8274,7 +8274,7 @@
         <v>20</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C232" t="s">
         <v>20</v>
@@ -8448,7 +8448,7 @@
         <v>20</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C238" t="s">
         <v>20</v>

</xml_diff>